<commit_message>
Arquivos com as análises do perfil aleatorio e tabela resumo de pontuação
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/Jogador que escolhe aleatoriamente/Tabela Resumo - Jogador que Escolhe Aleatoriamente - Base Completa.xlsx
+++ b/analises_dos_dados_preliminares/Jogador que escolhe aleatoriamente/Tabela Resumo - Jogador que Escolhe Aleatoriamente - Base Completa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\Jogador que escolhe aleatoriamente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C06272A-2B65-487A-BAAA-2E52B10E3AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58F7BC5-56E2-4F1F-B422-F5D139BB6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9A74655-EF3A-4D07-BF81-EB4937CE87C6}"/>
   </bookViews>
@@ -426,6 +426,120 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>100.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.039999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.82</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>63.289999999999992</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.93</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35.690000000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>35.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>56.69</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20.71</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30.09</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.52</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23.89</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.5100000000000011</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.4799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>51.339999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39.069999999999993</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -481,6 +595,120 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>106.17999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.839999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.699999999999989</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116.70000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.290000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>61.87</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26.919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.790000000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>67.989999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.39</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>51.790000000000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.35</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37.79</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>38.79</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.49</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.05</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>21.52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26.46</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>54.239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32.269999999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -536,6 +764,120 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>126.17999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.52000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.240000000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.079999999999984</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.47999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.02</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50.67</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45.629999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>46.160000000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30.79</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31.39</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41.09</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16.16</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32.049999999999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>97.95999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>56.95</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -764,6 +1106,120 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>46.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.539999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.89</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.279999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.92</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>51.69</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.93</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>36.36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>33.450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29.59</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>48.45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31.52</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38.14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17.04</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.5500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26.58</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1991,7 +2447,7 @@
   <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,162 +2634,390 @@
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4"/>
+      <c r="C3" s="4">
+        <v>100.88</v>
+      </c>
+      <c r="D3" s="4">
+        <v>53.039999999999992</v>
+      </c>
+      <c r="E3" s="4">
+        <v>67.14</v>
+      </c>
+      <c r="F3" s="4">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="G3" s="4">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="H3" s="4">
+        <v>71.13</v>
+      </c>
+      <c r="I3" s="4">
+        <v>68.84</v>
+      </c>
+      <c r="J3" s="4">
+        <v>90.84</v>
+      </c>
+      <c r="K3" s="4">
+        <v>78.52</v>
+      </c>
+      <c r="L3" s="4">
+        <v>55.25</v>
+      </c>
+      <c r="M3" s="4">
+        <v>60.1</v>
+      </c>
+      <c r="N3" s="4">
+        <v>49.41</v>
+      </c>
+      <c r="O3" s="4">
+        <v>5.07</v>
+      </c>
+      <c r="P3" s="4">
+        <v>17.27</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>48.680000000000007</v>
+      </c>
+      <c r="R3" s="4">
+        <v>38.82</v>
+      </c>
+      <c r="S3" s="4">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="T3" s="4">
+        <v>63.289999999999992</v>
+      </c>
+      <c r="U3" s="4">
+        <v>50.93</v>
+      </c>
+      <c r="V3" s="4">
+        <v>35.690000000000005</v>
+      </c>
+      <c r="W3" s="4">
+        <v>3.36</v>
+      </c>
+      <c r="X3" s="4">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>22.450000000000003</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>56.69</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>20.71</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>30.09</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>14.52</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>23.89</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>30.800000000000004</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>17.619999999999997</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>3.53</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>2.5100000000000011</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>5.16</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>6.4799999999999995</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>51.339999999999996</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>39.069999999999993</v>
+      </c>
       <c r="AO3" s="2">
         <f t="shared" ref="AO3:AO4" si="0">SUM(C3:AN3)</f>
-        <v>0</v>
+        <v>1406.4299999999996</v>
       </c>
       <c r="AP3" s="1">
         <v>6926.36</v>
       </c>
       <c r="AQ3" s="4">
         <f>(AO3*100)/$AP$3</f>
-        <v>0</v>
+        <v>20.305470694563951</v>
       </c>
     </row>
     <row r="4" spans="1:43" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
+      <c r="C4" s="4">
+        <v>106.17999999999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>58.839999999999996</v>
+      </c>
+      <c r="F4" s="4">
+        <v>18.13</v>
+      </c>
+      <c r="G4" s="4">
+        <v>81.699999999999989</v>
+      </c>
+      <c r="H4" s="4">
+        <v>116.70000000000002</v>
+      </c>
+      <c r="I4" s="4">
+        <v>29.290000000000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>104.54</v>
+      </c>
+      <c r="K4" s="4">
+        <v>53.22</v>
+      </c>
+      <c r="L4" s="4">
+        <v>128.25</v>
+      </c>
+      <c r="M4" s="4">
+        <v>47.11</v>
+      </c>
+      <c r="N4" s="4">
+        <v>34.53</v>
+      </c>
+      <c r="O4" s="4">
+        <v>11.34</v>
+      </c>
+      <c r="P4" s="4">
+        <v>61.87</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="R4" s="4">
+        <v>26.919999999999998</v>
+      </c>
+      <c r="S4" s="4">
+        <v>46.790000000000006</v>
+      </c>
+      <c r="T4" s="4">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="U4" s="4">
+        <v>12.39</v>
+      </c>
+      <c r="V4" s="4">
+        <v>51.790000000000006</v>
+      </c>
+      <c r="W4" s="4">
+        <v>2.76</v>
+      </c>
+      <c r="X4" s="4">
+        <v>26.7</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>27.35</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>4.09</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>37.79</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>38.79</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>2.4299999999999997</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>8.49</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>30.800000000000004</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>3.21</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>19.05</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>21.52</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>26.46</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>54.239999999999995</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>32.269999999999996</v>
+      </c>
       <c r="AO4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1440.9099999999999</v>
       </c>
       <c r="AP4" s="1">
         <v>7006.36</v>
       </c>
       <c r="AQ4" s="4">
         <f>(AO4*100)/$AP$4</f>
-        <v>0</v>
+        <v>20.565743124818024</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
+      <c r="C5" s="4">
+        <v>126.17999999999998</v>
+      </c>
+      <c r="D5" s="4">
+        <v>35.739999999999995</v>
+      </c>
+      <c r="E5" s="4">
+        <v>79.52000000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>91.240000000000009</v>
+      </c>
+      <c r="G5" s="4">
+        <v>91.079999999999984</v>
+      </c>
+      <c r="H5" s="4">
+        <v>99.93</v>
+      </c>
+      <c r="I5" s="4">
+        <v>7.59</v>
+      </c>
+      <c r="J5" s="4">
+        <v>77.47999999999999</v>
+      </c>
+      <c r="K5" s="4">
+        <v>64.52</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45.5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>27.21</v>
+      </c>
+      <c r="N5" s="4">
+        <v>14.030000000000001</v>
+      </c>
+      <c r="O5" s="4">
+        <v>27.54</v>
+      </c>
+      <c r="P5" s="4">
+        <v>7.07</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>67</v>
+      </c>
+      <c r="R5" s="4">
+        <v>27.02</v>
+      </c>
+      <c r="S5" s="4">
+        <v>2.17</v>
+      </c>
+      <c r="T5" s="4">
+        <v>50.67</v>
+      </c>
+      <c r="U5" s="4">
+        <v>45.629999999999995</v>
+      </c>
+      <c r="V5" s="4">
+        <v>46.160000000000004</v>
+      </c>
+      <c r="W5" s="4">
+        <v>2.56</v>
+      </c>
+      <c r="X5" s="4">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>22.450000000000003</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>30.79</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>31.39</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>18.12</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>41.09</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>16.16</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>32.300000000000004</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>15.120000000000001</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>14.25</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>12.120000000000001</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>97.95999999999998</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>56.95</v>
+      </c>
       <c r="AO5" s="2">
         <f>SUM(C5:AN5)</f>
-        <v>0</v>
+        <v>1539.2899999999997</v>
       </c>
       <c r="AP5" s="1">
         <v>6871.4599999999991</v>
       </c>
       <c r="AQ5" s="4">
         <f>(AO5*100)/$AP$5</f>
-        <v>0</v>
+        <v>22.401207312565305</v>
       </c>
     </row>
     <row r="6" spans="1:43" ht="30" x14ac:dyDescent="0.25">
@@ -2341,54 +3025,130 @@
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="12"/>
-      <c r="AJ6" s="12"/>
-      <c r="AK6" s="12"/>
-      <c r="AL6" s="12"/>
-      <c r="AM6" s="12"/>
-      <c r="AN6" s="12"/>
+      <c r="C6" s="12">
+        <v>46.17</v>
+      </c>
+      <c r="D6" s="12">
+        <v>72.539999999999992</v>
+      </c>
+      <c r="E6" s="12">
+        <v>47.04</v>
+      </c>
+      <c r="F6" s="12">
+        <v>29.73</v>
+      </c>
+      <c r="G6" s="12">
+        <v>22</v>
+      </c>
+      <c r="H6" s="12">
+        <v>72.53</v>
+      </c>
+      <c r="I6" s="12">
+        <v>63.04</v>
+      </c>
+      <c r="J6" s="12">
+        <v>54.08</v>
+      </c>
+      <c r="K6" s="12">
+        <v>33.22</v>
+      </c>
+      <c r="L6" s="12">
+        <v>2.81</v>
+      </c>
+      <c r="M6" s="12">
+        <v>52.01</v>
+      </c>
+      <c r="N6" s="12">
+        <v>14.030000000000001</v>
+      </c>
+      <c r="O6" s="12">
+        <v>5.07</v>
+      </c>
+      <c r="P6" s="12">
+        <v>55.89</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>30.279999999999998</v>
+      </c>
+      <c r="R6" s="12">
+        <v>9.92</v>
+      </c>
+      <c r="S6" s="12">
+        <v>3.5700000000000003</v>
+      </c>
+      <c r="T6" s="12">
+        <v>51.69</v>
+      </c>
+      <c r="U6" s="12">
+        <v>50.93</v>
+      </c>
+      <c r="V6" s="12">
+        <v>16.55</v>
+      </c>
+      <c r="W6" s="12">
+        <v>36.36</v>
+      </c>
+      <c r="X6" s="12">
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>19.490000000000002</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>29.59</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>48.45</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>31.52</v>
+      </c>
+      <c r="AD6" s="12">
+        <v>38.14</v>
+      </c>
+      <c r="AE6" s="12">
+        <v>17.04</v>
+      </c>
+      <c r="AF6" s="12">
+        <v>35</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>15.120000000000001</v>
+      </c>
+      <c r="AH6" s="12">
+        <v>5.5500000000000007</v>
+      </c>
+      <c r="AI6" s="12">
+        <v>12.120000000000001</v>
+      </c>
+      <c r="AJ6" s="12">
+        <v>4.25</v>
+      </c>
+      <c r="AK6" s="12">
+        <v>26.58</v>
+      </c>
+      <c r="AL6" s="12">
+        <v>3.05</v>
+      </c>
+      <c r="AM6" s="12">
+        <v>45.349999999999994</v>
+      </c>
+      <c r="AN6" s="12">
+        <v>2.0099999999999998</v>
+      </c>
       <c r="AO6" s="2">
         <f>SUM(C6:AN6)</f>
-        <v>0</v>
+        <v>1139.5699999999995</v>
       </c>
       <c r="AP6" s="6">
         <v>6666.2599999999966</v>
       </c>
       <c r="AQ6" s="4">
         <f>(AO6*100)/$AP$6</f>
-        <v>0</v>
+        <v>17.094592770158979</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
@@ -2526,17 +3286,17 @@
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="e">
+      <c r="B11" s="5">
         <f>AVERAGE(C3:AN3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="5" t="e">
+        <v>37.011315789473677</v>
+      </c>
+      <c r="D11" s="5">
         <f>STDEV(C3:AN3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" t="e">
+        <v>27.468212701825323</v>
+      </c>
+      <c r="F11">
         <f>(D11/B11*100)/100</f>
-        <v>#DIV/0!</v>
+        <v>0.74215715156059137</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="45" x14ac:dyDescent="0.25">
@@ -2551,17 +3311,17 @@
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="e">
+      <c r="B13" s="5">
         <f>AVERAGE(C4:AN4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D13" s="5" t="e">
+        <v>37.918684210526315</v>
+      </c>
+      <c r="D13" s="5">
         <f>STDEV(C4:AN4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" t="e">
+        <v>33.733130412268224</v>
+      </c>
+      <c r="F13">
         <f>(D13/B13*100)/100</f>
-        <v>#DIV/0!</v>
+        <v>0.88961764139758381</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="45" x14ac:dyDescent="0.25">
@@ -2576,17 +3336,17 @@
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="e">
+      <c r="B15" s="5">
         <f>AVERAGE(C5:AN5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="5" t="e">
+        <v>40.507631578947361</v>
+      </c>
+      <c r="D15" s="5">
         <f>STDEV(C5:AN5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" t="e">
+        <v>31.573621168602696</v>
+      </c>
+      <c r="F15">
         <f>(D15/B15*100)/100</f>
-        <v>#DIV/0!</v>
+        <v>0.77944870973429492</v>
       </c>
     </row>
     <row r="16" spans="1:43" ht="45" x14ac:dyDescent="0.25">
@@ -2601,17 +3361,17 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="e">
+      <c r="B17" s="5">
         <f>AVERAGE(C6:AN6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D17" s="5" t="e">
+        <v>29.988684210526301</v>
+      </c>
+      <c r="D17" s="5">
         <f>STDEV(C6:AN6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" t="e">
+        <v>20.736144468321374</v>
+      </c>
+      <c r="F17">
         <f>(D17/B17*100)/100</f>
-        <v>#DIV/0!</v>
+        <v>0.69146563159455998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>